<commit_message>
updated gitignore file and deleted target and test-output files
</commit_message>
<xml_diff>
--- a/src/main/resources/ClassDesignMapping.xlsx
+++ b/src/main/resources/ClassDesignMapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\serge\eclipse-workspace\Automation-testing\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{979EA272-F026-4CE3-ACEC-722917F75036}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BFBC60B-5089-47FF-B547-980C77C7B3FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{FC15B1E3-ECF4-4A67-AA52-3B6034C0300E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="42">
   <si>
     <t>BasePageObject</t>
   </si>
@@ -160,12 +160,6 @@
     <t xml:space="preserve"> -void setUpDriver(String browse, ITestContext ctx)</t>
   </si>
   <si>
-    <t>Webdriver driver;</t>
-  </si>
-  <si>
-    <t>Logger log</t>
-  </si>
-  <si>
     <t xml:space="preserve"> -void tearDown()</t>
   </si>
   <si>
@@ -197,6 +191,12 @@
   </si>
   <si>
     <t>ITestContext</t>
+  </si>
+  <si>
+    <t>WebDriver driver=new Webdriver();</t>
+  </si>
+  <si>
+    <t>Logger log=</t>
   </si>
 </sst>
 </file>
@@ -450,7 +450,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -473,6 +473,15 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2474,7 +2483,7 @@
   <dimension ref="A1:Q25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2482,7 +2491,7 @@
     <col min="1" max="4" width="8.7109375" customWidth="1"/>
     <col min="6" max="8" width="17.7109375" style="3"/>
     <col min="9" max="9" width="17.7109375" customWidth="1"/>
-    <col min="10" max="10" width="25.42578125" style="16" customWidth="1"/>
+    <col min="10" max="10" width="25.42578125" style="19" customWidth="1"/>
     <col min="11" max="11" width="9.85546875" style="3" customWidth="1"/>
     <col min="12" max="12" width="22" style="3" customWidth="1"/>
     <col min="13" max="13" width="6.42578125" style="3" customWidth="1"/>
@@ -2493,59 +2502,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J1" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="L1" s="45" t="s">
-        <v>41</v>
+      <c r="J1" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" s="48" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="44"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="47"/>
       <c r="F2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="N2" s="31" t="s">
+      <c r="N2" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="O2" s="32"/>
+      <c r="O2" s="35"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="41"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="44"/>
       <c r="F3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="17" t="s">
-        <v>37</v>
+      <c r="J3" s="20" t="s">
+        <v>35</v>
       </c>
       <c r="L3" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="N3" s="11" t="s">
-        <v>29</v>
+      <c r="N3" s="14" t="s">
+        <v>40</v>
       </c>
       <c r="O3" s="10"/>
     </row>
     <row r="4" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="24"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="27"/>
       <c r="F4" s="5" t="s">
         <v>23</v>
       </c>
@@ -2555,29 +2564,29 @@
       <c r="H4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J4" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="K4" s="14" t="s">
-        <v>39</v>
+      <c r="J4" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="K4" s="17" t="s">
+        <v>37</v>
       </c>
       <c r="L4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="N4" s="11" t="s">
-        <v>30</v>
+      <c r="N4" s="14" t="s">
+        <v>41</v>
       </c>
       <c r="O4" s="10"/>
     </row>
     <row r="5" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="40"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="41"/>
+      <c r="B5" s="43"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="44"/>
       <c r="E5" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>16</v>
@@ -2588,27 +2597,27 @@
       <c r="H5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J5" s="19" t="s">
+      <c r="J5" s="22" t="s">
         <v>24</v>
       </c>
       <c r="L5" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="N5" s="33" t="s">
+      <c r="N5" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="O5" s="34"/>
+      <c r="O5" s="37"/>
       <c r="P5" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="29"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="30"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="33"/>
       <c r="F6" s="5"/>
       <c r="G6" s="4" t="s">
         <v>16</v>
@@ -2616,61 +2625,61 @@
       <c r="H6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J6" s="20" t="s">
+      <c r="J6" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="N6" s="35" t="s">
+      <c r="N6" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="O6" s="36"/>
+      <c r="O6" s="39"/>
       <c r="Q6" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="29"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="30"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="33"/>
       <c r="H7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="J7" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="K7" s="12"/>
-      <c r="N7" s="37" t="s">
+      <c r="J7" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="O7" s="38"/>
+      <c r="K7" s="15"/>
+      <c r="N7" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="O7" s="41"/>
       <c r="Q7" s="6" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="29"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="30"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="33"/>
       <c r="F8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K8" s="13"/>
+      <c r="K8" s="16"/>
       <c r="Q8" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="29"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="30"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="33"/>
       <c r="F9" s="4" t="s">
         <v>5</v>
       </c>
@@ -2679,12 +2688,12 @@
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="28" t="s">
+      <c r="A10" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="29"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="30"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="33"/>
       <c r="F10" s="5" t="s">
         <v>23</v>
       </c>
@@ -2696,12 +2705,12 @@
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="29"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="30"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="33"/>
       <c r="F11" s="4" t="s">
         <v>16</v>
       </c>
@@ -2713,12 +2722,12 @@
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="29"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="30"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="33"/>
       <c r="G12" s="4" t="s">
         <v>16</v>
       </c>
@@ -2727,44 +2736,42 @@
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="29"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="30"/>
+      <c r="A13" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="13"/>
       <c r="H13" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="29"/>
-      <c r="C14" s="29"/>
-      <c r="D14" s="30"/>
+      <c r="A14" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="32"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="33"/>
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" s="29"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="30"/>
+      <c r="A15" s="31"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="33"/>
       <c r="F15" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="29"/>
-      <c r="C16" s="29"/>
-      <c r="D16" s="30"/>
+      <c r="A16" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="27"/>
       <c r="F16" s="5" t="s">
         <v>23</v>
       </c>
@@ -2774,12 +2781,12 @@
       <c r="H16" s="2"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="22" t="s">
+      <c r="A17" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="23"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="24"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="27"/>
       <c r="F17" s="4" t="s">
         <v>16</v>
       </c>
@@ -2791,12 +2798,12 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="22" t="s">
+      <c r="A18" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="23"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="24"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="27"/>
       <c r="G18" s="4" t="s">
         <v>16</v>
       </c>
@@ -2805,12 +2812,12 @@
       </c>
     </row>
     <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="25" t="s">
+      <c r="A19" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="26"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="27"/>
+      <c r="B19" s="29"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="30"/>
       <c r="H19" s="4" t="s">
         <v>16</v>
       </c>
@@ -2865,7 +2872,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="22">
+  <mergeCells count="21">
     <mergeCell ref="N2:O2"/>
     <mergeCell ref="N5:O5"/>
     <mergeCell ref="N6:O6"/>
@@ -2887,7 +2894,6 @@
     <mergeCell ref="A10:D10"/>
     <mergeCell ref="A11:D11"/>
     <mergeCell ref="A12:D12"/>
-    <mergeCell ref="A13:D13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>